<commit_message>
Microsoft Cloud Security Benchmark v1
</commit_message>
<xml_diff>
--- a/Microsoft Cloud Security Benchmark/Microsoft_cloud_security_benchmark_v1.xlsx
+++ b/Microsoft Cloud Security Benchmark/Microsoft_cloud_security_benchmark_v1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/chcheng1_microsoft_com/Documents/Multi-cloud/MCSB_v1_GA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1364" documentId="8_{68EA57A1-B688-4A17-B399-03A3CD93963D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DB88E6B-BAA5-45C6-B316-221BCA81D4C2}"/>
+  <xr:revisionPtr revIDLastSave="1366" documentId="8_{68EA57A1-B688-4A17-B399-03A3CD93963D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E996F4FA-F705-4A20-B8A0-34EA1048C711}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" tabRatio="786" xr2:uid="{30BFAFB3-652A-4F32-916F-A5B0C74C3635}"/>
   </bookViews>
@@ -1221,12 +1221,6 @@
     <t xml:space="preserve">Secured, isolated workstations are critically important for the security of sensitive roles like administrator, developer, and critical service operator.  </t>
   </si>
   <si>
-    <t>Understand privileged access workstations: 
-https://docs.microsoft.com/azure/active-directory/devices/concept-azure-managed-workstation
-Privileged access workstations deployment: 
-https://docs.microsoft.com/security/compass/privileged-access-deploymenthttps</t>
-  </si>
-  <si>
     <t>Use Session Manager in AWS Systems Manager to create an access path (a connection session) to the EC2 instance or a browser session to the AWS resources for privileged tasks. Session Manager allows RDP, SSH, and HTTPS connectivity to your destination hosts through port forwarding. 
 You may also choose to deploy a privileged access workstations (PAW) centrally managed through Azure Active Directory, Microsoft Defender, and/or Microsoft Intune. The central management should enforce secured configuration, including strong authentication, software and hardware baselines, and restricted logical and network access.</t>
   </si>
@@ -1821,12 +1815,6 @@
 https://docs.microsoft.com/azure/security/fundamentals/encryption-models
 Services that support encryption using customer-managed key: https://docs.microsoft.com/azure/security/fundamentals/encryption-models#supporting-services
 How to configure customer managed encryption keys in Azure Storage: https://docs.microsoft.com/azure/storage/common/storage-encryption-keys-portal</t>
-  </si>
-  <si>
-    <t>AWS Services Integrated with AWS KMS:
-https://aws.amazon.com/kms/features/
-AWS-managed and Customer-managed CMKs:
-https://docs.aws.amazon.com/whitepapers/latest/kms-best-practices/aws-managed-and-customer-managed-cmks.html</t>
   </si>
   <si>
     <t>SQL managed instances should use customer-managed keys to encrypt data at rest
@@ -6269,6 +6257,18 @@
       </rPr>
       <t xml:space="preserve">ntials, or service-linked roles to have a fine-grain control access control for your resources. </t>
     </r>
+  </si>
+  <si>
+    <t>AWS Services Integrated with AWS KMS:
+https://aws.amazon.com/kms/features/
+AWS-managed and Customer-managed CMKs:
+https://docs.aws.amazon.com/kms/latest/developerguide/concepts.html#key-mgmt</t>
+  </si>
+  <si>
+    <t>Understand privileged access workstations: 
+https://learn.microsoft.com/en-us/security/privileged-access-workstations/overview
+Privileged access workstations deployment: 
+https://docs.microsoft.com/security/compass/privileged-access-deploymenthttps</t>
   </si>
 </sst>
 </file>
@@ -6849,6 +6849,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7171,14 +7175,14 @@
     <row r="2" spans="1:4" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A2"/>
       <c r="B2" s="61" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C2" s="62"/>
     </row>
     <row r="3" spans="1:4" ht="118.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="B3" s="63" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C3" s="64"/>
     </row>
@@ -7375,125 +7379,125 @@
     </row>
     <row r="2" spans="1:13" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>550</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>554</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>556</v>
       </c>
       <c r="F2" s="5">
         <v>11.5</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="5" t="s">
         <v>558</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>559</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>560</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>885</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>561</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="221.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
+        <v>561</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>565</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F3" s="5">
         <v>5.0999999999999996</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>566</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="K3" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>567</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>568</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>886</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>569</v>
-      </c>
       <c r="M3" s="5" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>572</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="G4" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>575</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="K4" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>576</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>760</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>577</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>761</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>578</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
   </sheetData>
@@ -7575,166 +7579,166 @@
     </row>
     <row r="2" spans="1:13" ht="240" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>577</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="18" t="s">
         <v>581</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>583</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>94</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>584</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>585</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>887</v>
-      </c>
-      <c r="J2" s="10" t="s">
+      <c r="M2" s="5" t="s">
         <v>586</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>888</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>587</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
+        <v>587</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="18" t="s">
         <v>590</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>592</v>
       </c>
       <c r="F3" s="2">
         <v>3.4</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>593</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="M3" s="5" t="s">
         <v>594</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>889</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>759</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>890</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>595</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="231.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>94</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="10" t="s">
         <v>600</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="5" t="s">
         <v>601</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="L4" s="5" t="s">
         <v>602</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>603</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>604</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
+        <v>604</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="18" t="s">
         <v>607</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>609</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>94</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>610</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="K5" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="L5" s="10" t="s">
         <v>611</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>891</v>
-      </c>
-      <c r="J5" s="10" t="s">
+      <c r="M5" s="5" t="s">
         <v>612</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>891</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>613</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>614</v>
       </c>
     </row>
   </sheetData>
@@ -7800,13 +7804,13 @@
         <v>22</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="K1" s="24" t="s">
         <v>23</v>
       </c>
       <c r="L1" s="24" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="M1" s="24" t="s">
         <v>27</v>
@@ -7814,81 +7818,81 @@
     </row>
     <row r="2" spans="1:13" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>619</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>620</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="H2" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>622</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>892</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="M2" s="5" t="s">
         <v>624</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>893</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>625</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="361.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>625</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>618</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="5" t="s">
         <v>629</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>630</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="H3" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="I3" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>632</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="K3" s="9" t="s">
+        <v>893</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>633</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>894</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>634</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>895</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>635</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>178</v>
@@ -7896,81 +7900,81 @@
     </row>
     <row r="4" spans="1:13" ht="378" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>634</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>618</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>638</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="I4" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="K4" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>642</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>896</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="M4" s="5" t="s">
         <v>643</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>897</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>644</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="211.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>646</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>618</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>648</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>631</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="I5" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>650</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="K5" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>651</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>898</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>652</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>899</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>653</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>178</v>
@@ -7978,40 +7982,40 @@
     </row>
     <row r="6" spans="1:13" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>652</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>654</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>618</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>648</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>631</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="I6" s="7" t="s">
+        <v>898</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="K6" s="7" t="s">
+        <v>899</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>656</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>900</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>657</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>901</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>658</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>178</v>
@@ -8019,84 +8023,84 @@
     </row>
     <row r="7" spans="1:13" ht="310.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>657</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>659</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>618</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="G7" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>639</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="H7" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="I7" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="K7" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>664</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>902</v>
-      </c>
-      <c r="J7" s="2" t="s">
+      <c r="M7" s="5" t="s">
         <v>665</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>903</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>666</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>668</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>618</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>669</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="G8" s="5" t="s">
         <v>670</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="H8" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="I8" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="K8" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>673</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>905</v>
-      </c>
-      <c r="J8" s="2" t="s">
+      <c r="M8" s="5" t="s">
         <v>674</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>906</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>676</v>
       </c>
     </row>
   </sheetData>
@@ -8160,7 +8164,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="J1" s="23" t="s">
         <v>109</v>
@@ -8171,360 +8175,360 @@
     </row>
     <row r="2" spans="1:11" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
+        <v>676</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>680</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>681</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>682</v>
       </c>
       <c r="F2" s="12">
         <v>12.4</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>131</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>683</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>684</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>685</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>689</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="9" t="s">
         <v>690</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>692</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>131</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
+        <v>693</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>696</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>698</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>699</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>700</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>131</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="173.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
+        <v>701</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>704</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5" s="9" t="s">
         <v>706</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>707</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>708</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>131</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
+        <v>709</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="G6" s="9" t="s">
         <v>713</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>714</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>715</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>131</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
+        <v>715</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>717</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>718</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="G7" s="9" t="s">
         <v>720</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>721</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>722</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>131</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="330.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
+        <v>723</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>726</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="F8" s="9" t="s">
         <v>727</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="G8" s="9" t="s">
         <v>728</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>729</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>730</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>131</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="288" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
+        <v>731</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>733</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>735</v>
       </c>
       <c r="F9" s="12">
         <v>3.4</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>131</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="155.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
+        <v>737</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>739</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>740</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>741</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="G10" s="9" t="s">
         <v>742</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>743</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>744</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>131</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
+        <v>745</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>747</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>748</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>749</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="G11" s="9" t="s">
         <v>750</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>752</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>131</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>94</v>
@@ -8539,19 +8543,19 @@
         <v>94</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>131</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
   </sheetData>
@@ -8565,7 +8569,7 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8657,10 +8661,10 @@
         <v>35</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="J2" s="60" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="K2" s="57" t="s">
         <v>36</v>
@@ -8698,13 +8702,13 @@
         <v>44</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>45</v>
@@ -8739,13 +8743,13 @@
         <v>52</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>53</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>54</v>
@@ -8780,13 +8784,13 @@
         <v>61</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="J5" s="60" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>62</v>
@@ -8821,13 +8825,13 @@
         <v>69</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>70</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>71</v>
@@ -8862,13 +8866,13 @@
         <v>76</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>77</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>78</v>
@@ -8903,13 +8907,13 @@
         <v>83</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>84</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>85</v>
@@ -8944,13 +8948,13 @@
         <v>90</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>91</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>92</v>
@@ -8985,13 +8989,13 @@
         <v>98</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>99</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>100</v>
@@ -9026,13 +9030,13 @@
         <v>106</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>107</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>108</v>
@@ -9143,13 +9147,13 @@
         <v>117</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>118</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>119</v>
@@ -9184,13 +9188,13 @@
         <v>127</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>789</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>790</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>791</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>792</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>128</v>
@@ -9225,13 +9229,13 @@
         <v>133</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>134</v>
@@ -9266,13 +9270,13 @@
         <v>139</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>140</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>141</v>
@@ -9307,13 +9311,13 @@
         <v>147</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>148</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>149</v>
@@ -9348,13 +9352,13 @@
         <v>157</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>158</v>
       </c>
       <c r="K7" s="55" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>159</v>
@@ -9389,13 +9393,13 @@
         <v>165</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>166</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>167</v>
@@ -9430,13 +9434,13 @@
         <v>175</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>176</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>177</v>
@@ -9471,13 +9475,13 @@
         <v>184</v>
       </c>
       <c r="I10" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>804</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>806</v>
-      </c>
       <c r="K10" s="4" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>185</v>
@@ -9500,9 +9504,9 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J2" sqref="J2"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9589,13 +9593,13 @@
         <v>194</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>195</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>196</v>
@@ -9633,10 +9637,10 @@
         <v>202</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>203</v>
@@ -9671,13 +9675,13 @@
         <v>210</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>808</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>810</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>211</v>
@@ -9712,13 +9716,13 @@
         <v>218</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>219</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>220</v>
@@ -9753,13 +9757,13 @@
         <v>223</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>224</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>225</v>
@@ -9794,65 +9798,65 @@
         <v>232</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="J7" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="K7" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="L7" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="20" customFormat="1" ht="169.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>188</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>821</v>
-      </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="20" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>188</v>
@@ -9864,31 +9868,31 @@
         <v>206</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>94</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>820</v>
-      </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="6" t="s">
+        <v>817</v>
+      </c>
+      <c r="L9" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>819</v>
-      </c>
-      <c r="L9" s="9" t="s">
+      <c r="M9" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -9908,7 +9912,7 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J2" sqref="J2"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9971,7 +9975,7 @@
         <v>24</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N1" s="28" t="s">
         <v>25</v>
@@ -9980,7 +9984,7 @@
         <v>26</v>
       </c>
       <c r="P1" s="27" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="Q1" s="24" t="s">
         <v>27</v>
@@ -9988,245 +9992,245 @@
     </row>
     <row r="2" spans="1:17" ht="286.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>298</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>826</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>827</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>828</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="O2" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="P2" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>308</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="K3" s="59" t="s">
         <v>315</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>829</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>830</v>
-      </c>
-      <c r="K3" s="59" t="s">
+      <c r="L3" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="O3" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="Q3" s="5" t="s">
         <v>318</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="335.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>831</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>832</v>
-      </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="O4" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="P4" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="Q4" s="5" t="s">
         <v>331</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="216" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>834</v>
-      </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>833</v>
-      </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="O5" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="P5" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="P5" s="5" t="s">
-        <v>344</v>
-      </c>
       <c r="Q5" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="17" t="s">
+        <v>833</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>835</v>
-      </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>836</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>352</v>
-      </c>
       <c r="Q6" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>94</v>
@@ -10235,45 +10239,45 @@
         <v>94</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F7" s="11">
         <v>3.6</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>835</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="K7" s="14" t="s">
+        <v>836</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="I7" s="14" t="s">
-        <v>837</v>
-      </c>
-      <c r="J7" s="2" t="s">
+      <c r="M7" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="K7" s="14" t="s">
-        <v>838</v>
-      </c>
-      <c r="L7" s="5" t="s">
+      <c r="O7" s="10" t="s">
         <v>358</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="Q7" s="5" t="s">
         <v>359</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="291.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>94</v>
@@ -10282,45 +10286,45 @@
         <v>94</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F8" s="11">
         <v>3.6</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>840</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="K8" s="9" t="s">
+        <v>841</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>842</v>
-      </c>
-      <c r="J8" s="2" t="s">
+      <c r="M8" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="K8" s="9" t="s">
-        <v>843</v>
-      </c>
-      <c r="L8" s="5" t="s">
+      <c r="O8" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="M8" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>369</v>
-      </c>
       <c r="Q8" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>94</v>
@@ -10329,37 +10333,37 @@
         <v>94</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F9" s="11">
         <v>3.6</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>838</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>839</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="M9" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="I9" s="14" t="s">
-        <v>840</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>839</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>841</v>
-      </c>
-      <c r="L9" s="5" t="s">
+      <c r="O9" s="10" t="s">
         <v>373</v>
       </c>
-      <c r="M9" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="O9" s="10" t="s">
-        <v>375</v>
-      </c>
       <c r="Q9" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -10440,207 +10444,207 @@
     </row>
     <row r="2" spans="1:13" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>259</v>
       </c>
       <c r="F2" s="5">
         <v>2.4</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>849</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>850</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>263</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>267</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F3" s="5">
         <v>6.3</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>273</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="F4" s="5">
         <v>2.4</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>851</v>
-      </c>
-      <c r="J4" s="10" t="s">
+      <c r="K4" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>852</v>
-      </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>282</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>94</v>
       </c>
       <c r="G5" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>845</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>848</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>847</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>910</v>
-      </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>292</v>
       </c>
       <c r="F6" s="5">
         <v>6.3</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="J6" s="56" t="s">
+        <v>842</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="J6" s="56" t="s">
-        <v>844</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>295</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -10733,289 +10737,289 @@
     </row>
     <row r="2" spans="1:14" s="12" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>865</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>864</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>866</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="12" customFormat="1" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>862</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>863</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>391</v>
-      </c>
       <c r="N3" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="12" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="K4" s="7" t="s">
+        <v>856</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>860</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>858</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>399</v>
-      </c>
       <c r="N4" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="12" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>402</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F5" s="2">
         <v>10.8</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>763</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>859</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>765</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>857</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="12" customFormat="1" ht="249.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>409</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>94</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="K6" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>855</v>
-      </c>
-      <c r="J6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>856</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="12" customFormat="1" ht="216" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="I7" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>854</v>
-      </c>
-      <c r="J7" s="2" t="s">
+      <c r="L7" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>424</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="12" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>427</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>429</v>
       </c>
       <c r="F8" s="2">
         <v>10.4</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="K8" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>433</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>853</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -11097,133 +11101,133 @@
     </row>
     <row r="2" spans="1:13" s="20" customFormat="1" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="52" t="s">
         <v>438</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="E2" s="52" t="s">
-        <v>440</v>
       </c>
       <c r="F2" s="19">
         <v>10.8</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>867</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>868</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="52" t="s">
         <v>447</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="G3" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="H3" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="58" t="s">
         <v>451</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="I3" s="58" t="s">
+      <c r="K3" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>869</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="20" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="52" t="s">
         <v>458</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>460</v>
       </c>
       <c r="F4" s="19">
         <v>10.8</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>870</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>465</v>
-      </c>
       <c r="M4" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="20" customFormat="1" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>94</v>
@@ -11232,80 +11236,80 @@
         <v>94</v>
       </c>
       <c r="E5" s="52" t="s">
+        <v>465</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="I5" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="K5" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>876</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>877</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>471</v>
-      </c>
       <c r="M5" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="20" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>465</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="E6" s="52" t="s">
-        <v>467</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="I6" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>909</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>871</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>477</v>
-      </c>
       <c r="M6" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="20" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>94</v>
@@ -11314,72 +11318,72 @@
         <v>94</v>
       </c>
       <c r="E7" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="I7" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="K7" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>872</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>875</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>483</v>
-      </c>
       <c r="M7" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="2" customFormat="1" ht="178.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>94</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="I8" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="K8" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>873</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>874</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>490</v>
-      </c>
       <c r="M8" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -11461,289 +11465,289 @@
     </row>
     <row r="2" spans="1:13" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>494</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>497</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>878</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="M2" s="5" t="s">
         <v>499</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>879</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>500</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="205.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>502</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="H3" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="J3" s="56" t="s">
         <v>505</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="K3" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>880</v>
-      </c>
-      <c r="J3" s="56" t="s">
-        <v>507</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>881</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>508</v>
-      </c>
       <c r="M3" s="5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="172.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>513</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>882</v>
-      </c>
-      <c r="J4" s="9" t="s">
+      <c r="L4" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>517</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F5" s="5">
         <v>2.2000000000000002</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>905</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>519</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>883</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>907</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>908</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>521</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="271.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="H6" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="J6" s="9" t="s">
         <v>528</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="K6" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>529</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>530</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>884</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>531</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="232.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>534</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="H7" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="I7" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>537</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="K7" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>539</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>764</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>540</v>
-      </c>
       <c r="M7" s="5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="F8" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="H8" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="J8" s="9" t="s">
         <v>547</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="K8" s="5" t="s">
         <v>548</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="L8" s="5" t="s">
         <v>549</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>550</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>551</v>
-      </c>
       <c r="M8" s="5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -11753,6 +11757,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f7385881-037e-4b91-bb29-d3b325010731">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007C1E3484E1B71F4D99B2BD68D6237139" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f05dcfc413c1a45ea7464dcf13870a9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f7385881-037e-4b91-bb29-d3b325010731" xmlns:ns3="31336433-bca3-4ae1-849c-abc5b15f638f" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c1a0d26df6adf7959c3170cbb53aeaa6" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -11993,19 +12010,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f7385881-037e-4b91-bb29-d3b325010731">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -12016,6 +12020,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0E37C4-1EEA-4BE9-ADC7-FC5801053B93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f7385881-037e-4b91-bb29-d3b325010731"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC3D2014-BCB7-4C66-9627-CA383FCAC2D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12036,18 +12052,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0E37C4-1EEA-4BE9-ADC7-FC5801053B93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="f7385881-037e-4b91-bb29-d3b325010731"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96053E57-8459-4FD6-8F54-99848539D806}">
   <ds:schemaRefs>

</xml_diff>